<commit_message>
leading zeroes included in ID number,  df rearranged with mobile and linkedin included
</commit_message>
<xml_diff>
--- a/gecko_export_template.xlsx
+++ b/gecko_export_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameslay\Documents\GitHub\excel-manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9548138-DDD5-4681-BF75-80F84579EC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF40E70C-864D-4908-BFC4-F7C161335726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2475" windowWidth="21840" windowHeight="13140" xr2:uid="{5A14F905-4B0F-47A9-A9B1-DE04B62771FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Alumni number</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>SE1</t>
+  </si>
+  <si>
+    <t>000123456</t>
+  </si>
+  <si>
+    <t>000654321</t>
   </si>
 </sst>
 </file>
@@ -165,12 +171,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -489,18 +497,19 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="6"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -553,8 +562,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>123456</v>
+      <c r="A2" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -600,8 +609,8 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>654321</v>
+      <c r="A3" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>